<commit_message>
Fixed chart and added logarithmic version
</commit_message>
<xml_diff>
--- a/demo/Kaavioita.xlsx
+++ b/demo/Kaavioita.xlsx
@@ -1,517 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppp2/Documents/GitHub/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a9ea9677b856103/Distributed Systems 2022/GitHub/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC129B0D-E8CF-5E46-B816-F574B785BB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{FC129B0D-E8CF-5E46-B816-F574B785BB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A79A9324-6134-40FD-9491-B55663EC7A08}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="25440" windowHeight="14040" xr2:uid="{755D7349-032B-A148-871C-30EE62C7F95B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{755D7349-032B-A148-871C-30EE62C7F95B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.120" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.121" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.122" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.123" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.124" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.125" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.126" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.127" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.128" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.129" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.130" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.131" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.132" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.133" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.134" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.135" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.136" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.137" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.138" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.139" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.140" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.141" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.142" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.143" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.144" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.145" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.146" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.147" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.148" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.149" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.150" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.151" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.152" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.153" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.154" hidden="1">Sheet1!$C$26:$G$26</definedName>
-    <definedName name="_xlchart.v1.155" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.156" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.157" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.158" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.159" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.160" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.161" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.162" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.163" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.164" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.165" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.166" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.167" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.168" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.169" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.170" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.171" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.172" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.173" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.174" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.175" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.176" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.177" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.178" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.179" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.180" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.181" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.182" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.183" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.184" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.185" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.186" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.187" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.188" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.189" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.190" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.191" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.192" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.193" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.194" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.195" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.196" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.197" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.198" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.199" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.200" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.201" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.202" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.203" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.204" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.205" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.206" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.207" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.208" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.209" hidden="1">Sheet1!$C$26:$G$26</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.210" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.211" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.212" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.213" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.214" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.215" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.216" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.217" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.218" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.219" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.220" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.221" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.222" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.223" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.224" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.225" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.226" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.227" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.228" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.229" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.230" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.231" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.232" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.233" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.234" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.235" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.236" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.237" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.238" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.239" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.240" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.241" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.242" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.243" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.244" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.245" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.246" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.247" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.248" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.249" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.250" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.251" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.252" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.253" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.254" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.255" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.256" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.257" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.258" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.259" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.260" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.261" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.262" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.263" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.264" hidden="1">Sheet1!$C$26:$G$26</definedName>
-    <definedName name="_xlchart.v1.265" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.266" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.267" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.268" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.269" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.270" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.271" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.272" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.273" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.274" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.275" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.276" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.277" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.278" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.279" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.280" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.281" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.282" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.283" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.284" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.285" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.286" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.287" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.288" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.289" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.290" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.291" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.292" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.293" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.294" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.295" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.296" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.297" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.298" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.299" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.300" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.301" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.302" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.303" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.304" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.305" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.306" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.307" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.308" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.309" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.310" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.311" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.312" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.313" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.314" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.315" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.316" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.317" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.318" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.319" hidden="1">Sheet1!$C$26:$G$26</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.320" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.321" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.322" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.323" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.324" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.325" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.326" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.327" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.328" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.329" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.330" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.331" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.332" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.333" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.334" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.335" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.336" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.337" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.338" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.339" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.340" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.341" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.342" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.343" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.344" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.345" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.346" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.347" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.348" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.349" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.350" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.351" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.352" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.353" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.354" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.355" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.356" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.357" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.358" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.359" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.360" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.361" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.362" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.363" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.364" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.365" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.366" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.367" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.368" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.369" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.370" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.371" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.372" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.373" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.374" hidden="1">Sheet1!$C$26:$G$26</definedName>
-    <definedName name="_xlchart.v1.375" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.376" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.377" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.378" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.379" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.380" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.381" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.382" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.383" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.384" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.385" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.386" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.387" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.388" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.389" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.390" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.391" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.392" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.393" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.394" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.395" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.396" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.397" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.398" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.399" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.400" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.401" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.402" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.403" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.404" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.405" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.406" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.407" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.408" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.409" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.410" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.411" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.412" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.413" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.414" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.415" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.416" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.417" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.418" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.419" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.420" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.421" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.422" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.423" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.424" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.425" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.426" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.427" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.428" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.429" hidden="1">Sheet1!$C$26:$G$26</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.430" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.431" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.432" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.433" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.434" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.435" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.436" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.437" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.438" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.439" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$C$26:$G$26</definedName>
-    <definedName name="_xlchart.v1.440" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.441" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.442" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.443" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.444" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.445" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.446" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.447" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.448" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.449" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.450" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.451" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.452" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.453" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.454" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.455" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.456" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.457" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.458" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.459" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.460" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.461" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.462" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.463" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.464" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.465" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.466" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.467" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.468" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.469" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.470" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.471" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.472" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.473" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.474" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.475" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.476" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.477" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.478" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.479" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.480" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.481" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.482" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.483" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.484" hidden="1">Sheet1!$C$26:$G$26</definedName>
-    <definedName name="_xlchart.v1.485" hidden="1">Sheet1!$C$27:$G$27</definedName>
-    <definedName name="_xlchart.v1.486" hidden="1">Sheet1!$C$28:$G$28</definedName>
-    <definedName name="_xlchart.v1.487" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.488" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.489" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.490" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.491" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.492" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.493" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.494" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$C$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$C$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$C$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$C$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">Sheet1!$C$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">Sheet1!$C$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">Sheet1!$C$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">Sheet1!$C$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">Sheet1!$C$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">Sheet1!$C$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">Sheet1!$C$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">Sheet1!$C$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">Sheet1!$C$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">Sheet1!$C$20:$G$20</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">Sheet1!$C$21:$G$21</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">Sheet1!$C$22:$G$22</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">Sheet1!$C$23:$G$23</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">Sheet1!$C$24:$G$24</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">Sheet1!$C$25:$G$25</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">Sheet1!$C$26:$G$26</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -531,93 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>Mittauksiin meni  534.6032197</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>0 workers</t>
-  </si>
-  <si>
-    <t>1 workers</t>
-  </si>
-  <si>
-    <t>2 workers</t>
-  </si>
-  <si>
-    <t>3 workers</t>
-  </si>
-  <si>
-    <t>4 workers</t>
-  </si>
-  <si>
-    <t>5 workers</t>
-  </si>
-  <si>
-    <t>6 workers</t>
-  </si>
-  <si>
-    <t>7 workers</t>
-  </si>
-  <si>
-    <t>8 workers</t>
-  </si>
-  <si>
-    <t>9 workers</t>
-  </si>
-  <si>
-    <t>10 workers</t>
-  </si>
-  <si>
-    <t>11 workers</t>
-  </si>
-  <si>
-    <t>12 workers</t>
-  </si>
-  <si>
-    <t>13 workers</t>
-  </si>
-  <si>
-    <t>14 workers</t>
-  </si>
-  <si>
-    <t>15 workers</t>
-  </si>
-  <si>
-    <t>16 workers</t>
-  </si>
-  <si>
-    <t>17 workers</t>
-  </si>
-  <si>
-    <t>18 workers</t>
-  </si>
-  <si>
-    <t>19 workers</t>
-  </si>
-  <si>
-    <t>20 workers</t>
-  </si>
-  <si>
-    <t>21 workers</t>
-  </si>
-  <si>
-    <t>22 workers</t>
-  </si>
-  <si>
-    <t>23 workers</t>
-  </si>
-  <si>
-    <t>24 workers</t>
-  </si>
-  <si>
-    <t>25 workers</t>
-  </si>
-  <si>
-    <t>26 workers</t>
   </si>
   <si>
     <t>Case 0</t>
@@ -634,14 +56,17 @@
   <si>
     <t>Case 4</t>
   </si>
+  <si>
+    <t>Workers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="0.0000000E+00"/>
-    <numFmt numFmtId="181" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -681,8 +106,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,7 +128,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -721,7 +146,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -734,9 +159,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Execution times by in each case as a function of increasing worker count</a:t>
             </a:r>
+            <a:endParaRPr lang="en-FI" sz="1800">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -753,7 +183,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -772,8 +202,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -790,7 +220,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -813,96 +243,97 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
-            <c:strRef>
+          <c:cat>
+            <c:numRef>
               <c:f>Sheet1!$B$2:$B$28</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0 workers</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1 workers</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2 workers</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3 workers</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4 workers</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5 workers</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6 workers</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7 workers</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8 workers</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9 workers</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10 workers</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11 workers</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12 workers</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13 workers</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14 workers</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15 workers</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16 workers</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17 workers</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18 workers</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19 workers</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20 workers</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21 workers</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22 workers</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23 workers</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24 workers</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25 workers</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26 workers</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$28</c:f>
               <c:numCache>
@@ -991,11 +422,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F95A-0A4A-B53A-DB640EFDF5E4}"/>
+              <c16:uniqueId val="{00000000-2B9D-435A-AA70-F54D1F7ECA19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1014,7 +445,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1037,96 +468,97 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
-            <c:strRef>
+          <c:cat>
+            <c:numRef>
               <c:f>Sheet1!$B$2:$B$28</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0 workers</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1 workers</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2 workers</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3 workers</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4 workers</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5 workers</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6 workers</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7 workers</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8 workers</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9 workers</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10 workers</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11 workers</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12 workers</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13 workers</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14 workers</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15 workers</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16 workers</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17 workers</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18 workers</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19 workers</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20 workers</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21 workers</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22 workers</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23 workers</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24 workers</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25 workers</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26 workers</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$28</c:f>
               <c:numCache>
@@ -1215,11 +647,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F95A-0A4A-B53A-DB640EFDF5E4}"/>
+              <c16:uniqueId val="{00000001-2B9D-435A-AA70-F54D1F7ECA19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1238,7 +670,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -1261,96 +693,97 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
-            <c:strRef>
+          <c:cat>
+            <c:numRef>
               <c:f>Sheet1!$B$2:$B$28</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0 workers</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1 workers</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2 workers</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3 workers</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4 workers</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5 workers</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6 workers</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7 workers</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8 workers</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9 workers</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10 workers</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11 workers</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12 workers</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13 workers</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14 workers</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15 workers</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16 workers</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17 workers</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18 workers</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19 workers</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20 workers</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21 workers</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22 workers</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23 workers</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24 workers</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25 workers</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26 workers</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$28</c:f>
               <c:numCache>
@@ -1439,11 +872,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F95A-0A4A-B53A-DB640EFDF5E4}"/>
+              <c16:uniqueId val="{00000002-2B9D-435A-AA70-F54D1F7ECA19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1462,7 +895,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -1485,96 +918,97 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
-            <c:strRef>
+          <c:cat>
+            <c:numRef>
               <c:f>Sheet1!$B$2:$B$28</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0 workers</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1 workers</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2 workers</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3 workers</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4 workers</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5 workers</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6 workers</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7 workers</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8 workers</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9 workers</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10 workers</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11 workers</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12 workers</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13 workers</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14 workers</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15 workers</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16 workers</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17 workers</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18 workers</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19 workers</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20 workers</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21 workers</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22 workers</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23 workers</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24 workers</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25 workers</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26 workers</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$2:$F$28</c:f>
               <c:numCache>
@@ -1663,11 +1097,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F95A-0A4A-B53A-DB640EFDF5E4}"/>
+              <c16:uniqueId val="{00000003-2B9D-435A-AA70-F54D1F7ECA19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1686,7 +1120,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -1709,96 +1143,97 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
-            <c:strRef>
+          <c:cat>
+            <c:numRef>
               <c:f>Sheet1!$B$2:$B$28</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0 workers</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1 workers</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2 workers</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3 workers</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4 workers</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5 workers</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6 workers</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7 workers</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8 workers</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9 workers</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10 workers</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11 workers</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12 workers</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13 workers</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14 workers</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15 workers</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16 workers</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17 workers</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18 workers</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19 workers</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20 workers</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21 workers</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22 workers</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23 workers</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24 workers</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25 workers</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26 workers</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$G$2:$G$28</c:f>
               <c:numCache>
@@ -1887,11 +1322,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F95A-0A4A-B53A-DB640EFDF5E4}"/>
+              <c16:uniqueId val="{00000004-2B9D-435A-AA70-F54D1F7ECA19}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1903,30 +1338,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1478217679"/>
-        <c:axId val="1501345983"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1478217679"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1147694095"/>
+        <c:axId val="1147672463"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1147694095"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1947,12 +1370,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Number of workers (0 means</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> plain function without Pystributor)</a:t>
+                  <a:rPr lang="fi-FI"/>
+                  <a:t>Number of workers (0 means plain function without Pystributor)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1995,8 +1414,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2023,12 +1442,1534 @@
             <a:endParaRPr lang="en-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1501345983"/>
+        <c:crossAx val="1147672463"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1147672463"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fi-FI"/>
+                  <a:t>Time, seconds</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fi-FI" baseline="0"/>
+                  <a:t> log10</a:t>
+                </a:r>
+                <a:endParaRPr lang="fi-FI"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1147694095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fi-FI"/>
+              <a:t>Execution times by in each case as a function of increasing worker count</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Case 0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.1482377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>321.99298439999899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>173.66989029999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86.044696400000205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.440421400000503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.825848399999799</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.2092195</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1519753999999693</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.16727869999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.1754249000000501</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.1650836000001101</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.1772094999998899</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.1851584999999396</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1307822999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.64194800000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.6444083999999699</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6609425000000302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1699664000000198</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.1679183999999601</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.1782077999998801</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.6475482000000699</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1500442999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.7067316999999704</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.7911245999999803</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2316074000000299</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.1659166999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.1787891000000101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C070-45BA-93EB-F9681445ABCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Case 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>1.9805321499999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.3933415999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.260071200000301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1835068999998803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.17274999999972</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.65013869999984</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1309705000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5858102999999901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0992026000000101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.12045949999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6008115000001899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.60687430000007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6174335000000599</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1683827</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.63651820000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.65791000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1536327000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.66251860000011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.6653713000000601</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1687234000000899</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.6694961000000601</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1792340999999902</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.1950161000000299</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.7048902000000199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.2245180999999499</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.71888849999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2000257999999899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C070-45BA-93EB-F9681445ABCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Case 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>16.039719599999898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.867196199999803</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.270045000000199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.207414199999199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.2031372000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6885529999999491</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.1500872999999903</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6377866999999897</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.1346000999999397</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1404526000001098</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.6291381000000902</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1365321000000597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.1747126000000199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9398919999999897</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.68366049999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.70939740000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7433495000000203</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.6676723000000404</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.2337863999998699</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.81624450000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.2267102000000696</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.8638918999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.7336816999999698</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.8300145000000603</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.3824826999999598</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.0928082000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.8197708000000103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C070-45BA-93EB-F9681445ABCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Case 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>141.6770449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184.70040329999901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91.7696650999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66.015988699999895</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.452943600000197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.358884600000202</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.5429963999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.538352400000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.5485069</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.676265800000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.6210773</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.724978399999799</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.740849299999802</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.6728299</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28.702154699999902</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.572583999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.0033204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27.967914099999899</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29.123915299999901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.284465499999801</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26.7381554</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>27.762565800000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27.785947899999901</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>28.4684060999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.368732300000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28.525299799999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.9955704999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C070-45BA-93EB-F9681445ABCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Case 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>1282.5159466</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1483.80155609999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>680.19178749999901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>494.65283439999899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>445.69864249999898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>341.0752162</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>331.57242789999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>282.89193349999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>287.05257649999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>261.41194139999902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>235.09331879999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>238.335006499999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>238.95533549999899</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>239.164259299999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>237.30217060000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>233.09885070000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>227.94494589999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>235.09933000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>229.2615691</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>225.6642646</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>231.43178169999899</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>225.7574984</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>228.956696399999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230.6937461</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>219.51268580000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>227.77608979999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>231.55187659999899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C070-45BA-93EB-F9681445ABCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1217248111"/>
+        <c:axId val="1217262255"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1217248111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fi-FI"/>
+                  <a:t>Number of workers (0 means plain function without Pystributor)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1217262255"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="1501345983"/>
+        <c:axId val="1217262255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2068,7 +3009,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="fi-FI"/>
                   <a:t>Time (seconds)</a:t>
                 </a:r>
               </a:p>
@@ -2109,14 +3050,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2140,9 +3075,9 @@
             <a:endParaRPr lang="en-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1478217679"/>
+        <c:crossAx val="1217248111"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2267,8 +3202,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2295,8 +3270,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2397,7 +3372,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2429,10 +3404,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2472,23 +3447,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2593,8 +3567,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2726,12 +3700,302 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -2742,28 +4006,229 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
+  </cs:errorBar>
+  <cs:floor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2787,23 +4252,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>416394</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>83279</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>8660</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>184727</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>173675</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>206239</xdr:rowOff>
+      <xdr:colOff>23091</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>184728</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60620D22-15EF-0E48-9880-1ED5DF7A02A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32B33D63-9BC6-461B-9DD7-95264AD4237B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2816,6 +4281,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5774</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>13854</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57727</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C17F5DE9-9677-4CB4-A15C-2858F1077E03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3123,11 +4624,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199FDC45-C97B-C544-852E-61F7BDAB02A8}">
   <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="39" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" customWidth="1"/>
@@ -3138,26 +4639,29 @@
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <v>0.1482377</v>
@@ -3175,9 +4679,9 @@
         <v>1282.5159466</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>3</v>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" s="3">
         <v>321.99298439999899</v>
@@ -3195,9 +4699,9 @@
         <v>1483.80155609999</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>4</v>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>2</v>
       </c>
       <c r="C4" s="3">
         <v>173.66989029999999</v>
@@ -3215,9 +4719,9 @@
         <v>680.19178749999901</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>5</v>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>86.044696400000205</v>
@@ -3235,9 +4739,9 @@
         <v>494.65283439999899</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>6</v>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>4</v>
       </c>
       <c r="C6" s="3">
         <v>37.440421400000503</v>
@@ -3255,9 +4759,9 @@
         <v>445.69864249999898</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>7</v>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>5</v>
       </c>
       <c r="C7" s="3">
         <v>20.825848399999799</v>
@@ -3275,9 +4779,9 @@
         <v>341.0752162</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>8</v>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>6</v>
       </c>
       <c r="C8" s="3">
         <v>16.2092195</v>
@@ -3298,9 +4802,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>9</v>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>7</v>
       </c>
       <c r="C9" s="3">
         <v>8.1519753999999693</v>
@@ -3321,9 +4825,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>10</v>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>8.16727869999999</v>
@@ -3344,9 +4848,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>11</v>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>9</v>
       </c>
       <c r="C11" s="3">
         <v>7.1754249000000501</v>
@@ -3367,9 +4871,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>12</v>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>5.1650836000001101</v>
@@ -3390,9 +4894,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>13</v>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>11</v>
       </c>
       <c r="C13" s="3">
         <v>5.1772094999998899</v>
@@ -3413,9 +4917,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>14</v>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>12</v>
       </c>
       <c r="C14" s="3">
         <v>4.1851584999999396</v>
@@ -3433,9 +4937,9 @@
         <v>238.95533549999899</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>15</v>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>13</v>
       </c>
       <c r="C15" s="3">
         <v>2.1307822999999999</v>
@@ -3456,9 +4960,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>16</v>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>14</v>
       </c>
       <c r="C16" s="3">
         <v>2.64194800000001</v>
@@ -3479,9 +4983,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>17</v>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>15</v>
       </c>
       <c r="C17" s="3">
         <v>2.6444083999999699</v>
@@ -3502,9 +5006,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>18</v>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>16</v>
       </c>
       <c r="C18" s="3">
         <v>2.6609425000000302</v>
@@ -3525,9 +5029,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>19</v>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>17</v>
       </c>
       <c r="C19" s="3">
         <v>3.1699664000000198</v>
@@ -3548,9 +5052,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>20</v>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>18</v>
       </c>
       <c r="C20" s="3">
         <v>3.1679183999999601</v>
@@ -3571,9 +5075,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>21</v>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>19</v>
       </c>
       <c r="C21" s="3">
         <v>3.1782077999998801</v>
@@ -3594,9 +5098,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>22</v>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>20</v>
       </c>
       <c r="C22" s="3">
         <v>2.6475482000000699</v>
@@ -3614,9 +5118,9 @@
         <v>231.43178169999899</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>23</v>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>21</v>
       </c>
       <c r="C23" s="3">
         <v>2.1500442999999998</v>
@@ -3637,9 +5141,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>24</v>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>22</v>
       </c>
       <c r="C24" s="3">
         <v>4.7067316999999704</v>
@@ -3660,9 +5164,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>25</v>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>23</v>
       </c>
       <c r="C25" s="3">
         <v>5.7911245999999803</v>
@@ -3683,9 +5187,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>26</v>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>24</v>
       </c>
       <c r="C26" s="3">
         <v>3.2316074000000299</v>
@@ -3703,9 +5207,9 @@
         <v>219.51268580000001</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>27</v>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>25</v>
       </c>
       <c r="C27" s="3">
         <v>2.1659166999999999</v>
@@ -3726,9 +5230,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>28</v>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>26</v>
       </c>
       <c r="C28" s="3">
         <v>3.1787891000000101</v>
@@ -3746,15 +5250,15 @@
         <v>231.55187659999899</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D38" s="1"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -3762,7 +5266,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -3770,7 +5274,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -3778,7 +5282,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -3786,7 +5290,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -3794,7 +5298,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -3802,7 +5306,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -3810,7 +5314,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -3818,7 +5322,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -3826,7 +5330,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -3834,7 +5338,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -3842,7 +5346,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -3850,7 +5354,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -3858,7 +5362,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -3866,7 +5370,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -3874,7 +5378,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -3882,7 +5386,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -3890,7 +5394,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -3898,7 +5402,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -3906,7 +5410,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -3914,7 +5418,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -3922,7 +5426,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -3930,7 +5434,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -3938,7 +5442,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -3946,7 +5450,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -3954,7 +5458,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -3962,7 +5466,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>

</xml_diff>